<commit_message>
added extra colums for prediction to calculate % of win or relegate, preparing for monte carlo symulation
</commit_message>
<xml_diff>
--- a/Prediction/Ekstraklasa2025_26/Predicted_Ekstraklasa2025_26_table_matchday_0.xlsx
+++ b/Prediction/Ekstraklasa2025_26/Predicted_Ekstraklasa2025_26_table_matchday_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,26 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>WIN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>TOP2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>TOP4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>RELEGATION</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>ExpPoints</t>
         </is>
       </c>
@@ -459,7 +479,11 @@
           <t>Raków Częstochowa</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>59.32702618632252</v>
       </c>
     </row>
@@ -472,7 +496,11 @@
           <t>Jagiellonia Białystok</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
         <v>56.24885845706865</v>
       </c>
     </row>
@@ -485,7 +513,11 @@
           <t>Lech Poznań</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
         <v>51.93951623443239</v>
       </c>
     </row>
@@ -498,7 +530,11 @@
           <t>Górnik Zabrze</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
         <v>51.3705476798805</v>
       </c>
     </row>
@@ -511,7 +547,11 @@
           <t>Legia Warszawa</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
         <v>49.46067869752017</v>
       </c>
     </row>
@@ -524,7 +564,11 @@
           <t>Cracovia</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
         <v>47.63627167701561</v>
       </c>
     </row>
@@ -537,7 +581,11 @@
           <t>Pogoń Szczecin</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="n">
         <v>46.37886332263477</v>
       </c>
     </row>
@@ -550,7 +598,11 @@
           <t>Wisła Płock</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="n">
         <v>44.91281723624755</v>
       </c>
     </row>
@@ -563,7 +615,11 @@
           <t>Korona Kielce</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
         <v>44.09707190291329</v>
       </c>
     </row>
@@ -576,7 +632,11 @@
           <t>Radomiak Radom</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="n">
         <v>43.60184648674157</v>
       </c>
     </row>
@@ -589,7 +649,11 @@
           <t>Zagłębie Lubin</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
         <v>42.91621342752069</v>
       </c>
     </row>
@@ -602,7 +666,11 @@
           <t>Piast Gliwice</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
         <v>42.03941238071236</v>
       </c>
     </row>
@@ -615,7 +683,11 @@
           <t>GKS Katowice</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
         <v>40.9810000648459</v>
       </c>
     </row>
@@ -628,7 +700,11 @@
           <t>Motor Lublin</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="n">
         <v>39.63152146311909</v>
       </c>
     </row>
@@ -641,7 +717,11 @@
           <t>Lechia Gdańsk</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
         <v>38.93203295975129</v>
       </c>
     </row>
@@ -654,7 +734,11 @@
           <t>Arka Gdynia</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>38.82679109312276</v>
       </c>
     </row>
@@ -667,7 +751,11 @@
           <t>Widzew Łódź</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="n">
         <v>38.20742140605261</v>
       </c>
     </row>
@@ -680,7 +768,11 @@
           <t>Nieciecza</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="n">
         <v>35.16283873610946</v>
       </c>
     </row>

</xml_diff>